<commit_message>
Added some fixes to display time as hh:mm in the report.
</commit_message>
<xml_diff>
--- a/data/time_template.xlsx
+++ b/data/time_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\sword\attendance-analyzer\attendanceAnalyzer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wael\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{BEE672A6-2B0E-45C1-A3A2-A6321719B8FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{2FFA6B97-248F-4401-9745-FE70D4198AE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21615" windowHeight="7485" activeTab="1" xr2:uid="{5805C235-7555-469B-9EC8-AE310B4EA644}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -71,11 +71,20 @@
   <si>
     <t>Sum of Expected</t>
   </si>
+  <si>
+    <t>05/02/2019</t>
+  </si>
+  <si>
+    <t>05/03/2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,16 +157,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -325,10 +335,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1/3/1900</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1/4/1900</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -340,17 +350,17 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>9.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>4.9400000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C2B9-4CE0-A2B6-45B2ADA235EC}"/>
+              <c16:uniqueId val="{00000000-990F-4E1B-BDA1-6111CCD1D779}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -401,10 +411,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1/3/1900</c:v>
+                  <c:v>05/02/2019</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1/4/1900</c:v>
+                  <c:v>05/03/2019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -416,10 +426,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,7 +437,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C2B9-4CE0-A2B6-45B2ADA235EC}"/>
+              <c16:uniqueId val="{00000001-990F-4E1B-BDA1-6111CCD1D779}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1197,23 +1207,25 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Wael" refreshedDate="43600.369550694442" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13" xr:uid="{C7C69103-0374-49FC-8D10-4171FCAD41D0}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Wael" refreshedDate="43616.355554398149" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13" xr:uid="{C7C69103-0374-49FC-8D10-4171FCAD41D0}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C1048576" sheet="DATA"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1900-01-02T00:00:00" maxDate="1900-01-04T00:00:00" count="3">
-        <d v="1900-01-02T00:00:00"/>
-        <d v="1900-01-03T00:00:00"/>
+      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="1900-01-02T00:00:00" maxDate="1900-01-04T00:00:00" count="5">
+        <s v="05/02/2019"/>
+        <s v="05/03/2019"/>
         <m/>
+        <d v="1900-01-03T00:00:00" u="1"/>
+        <d v="1900-01-02T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Actual" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.9400000000000004" maxValue="9.64"/>
     </cacheField>
     <cacheField name="Expected" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="9" maxValue="9"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1228,13 +1240,13 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="13">
   <r>
     <x v="0"/>
-    <n v="3"/>
-    <n v="3"/>
+    <n v="9.64"/>
+    <n v="9"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="4"/>
-    <n v="4"/>
+    <n v="4.9400000000000004"/>
+    <n v="9"/>
   </r>
   <r>
     <x v="2"/>
@@ -1295,12 +1307,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BAD40493-5B73-4185-BE5E-44BCE9254DDA}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="27" rowHeaderCaption="Date">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BAD40493-5B73-4185-BE5E-44BCE9254DDA}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="27" rowHeaderCaption="Date">
   <location ref="A1:C3" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" measureFilter="1">
-      <items count="4">
+      <items count="6">
         <item x="2"/>
+        <item m="1" x="4"/>
+        <item m="1" x="3"/>
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
@@ -1314,10 +1328,10 @@
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="1"/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="4"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -2146,7 +2160,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A2:C3"/>
+      <selection activeCell="A3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,29 +2185,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -2218,19 +2213,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2248,39 +2243,39 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>3</v>
-      </c>
-      <c r="B2" s="9">
-        <v>3</v>
-      </c>
-      <c r="C2" s="9">
-        <v>3</v>
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10">
+        <v>9.64</v>
+      </c>
+      <c r="C2" s="10">
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="5">
         <f>DATA!G2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>4</v>
-      </c>
-      <c r="B3" s="9">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9">
-        <v>4</v>
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="C3" s="10">
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3">
         <f>SUM(B:B)</f>
-        <v>7</v>
+        <v>14.580000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2289,15 +2284,15 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(C:C)</f>
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="str">
-        <f>IF(F3&gt;F4, F3-F4, "")</f>
+      <c r="F5" s="6" t="str">
+        <f>IF(F3&gt;F4, (F3-F4)/24, "")</f>
         <v/>
       </c>
     </row>
@@ -2305,18 +2300,18 @@
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4" t="str">
-        <f>IF(F3&lt;F4, F4-F3, "")</f>
-        <v/>
+      <c r="F6" s="7">
+        <f>IF(F3&lt;F4, (F4-F3)/24, "")</f>
+        <v>0.14249999999999993</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5">
-        <f>ROUND(F3/(COUNTA(B:B) -1),2)</f>
-        <v>3.5</v>
+      <c r="F7" s="8">
+        <f>ROUND(F3/(COUNTA(B:B) -1),2)/24</f>
+        <v>0.30375000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>